<commit_message>
Image and 3D hadling
</commit_message>
<xml_diff>
--- a/clients/python/dataspace-excel/Test.xlsx
+++ b/clients/python/dataspace-excel/Test.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\dataspace\clients\python\dataspace-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A483CB3-2753-4227-8984-1CAB9AF35E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748BF7B3-A196-41FA-A393-0999A5727177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13230" yWindow="90" windowWidth="32625" windowHeight="20070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14175" yWindow="870" windowWidth="37425" windowHeight="19110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -144,7 +143,7 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="xloil.6yl2gotp0ph6dlm1gluqvd">
+    <main first="xloil.69y1plpjwasixfgsbki47c">
       <tp>
         <v>0</v>
         <stp/>
@@ -427,7 +426,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>1073 W</a:t>
+            <a:t>1023 W</a:t>
           </a:fld>
           <a:endParaRPr lang="sv-SE" sz="2400"/>
         </a:p>
@@ -460,7 +459,7 @@
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
-        <a:xfrm rot="-6240857">
+        <a:xfrm rot="-6369429">
           <a:off x="15471539" y="11985958"/>
           <a:ext cx="193942" cy="2787917"/>
           <a:chOff x="10791825" y="11544300"/>
@@ -560,6 +559,187 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:am3d="http://schemas.microsoft.com/office/drawing/2017/model3d" Requires="am3d">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="mqtt://iot.digivis.se/datadirectory/TestArea/TestFiles/monkey.glb">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7D9A5B7-D57E-02FA-75CB-B9F1C91C95C2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr>
+              <a:graphicFrameLocks noChangeAspect="1"/>
+            </xdr:cNvGraphicFramePr>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2017/model3d">
+              <am3d:model3d xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" r:link="rId3">
+                <am3d:spPr>
+                  <a:xfrm>
+                    <a:off x="0" y="0"/>
+                    <a:ext cx="1885950" cy="1409700"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                </am3d:spPr>
+                <am3d:camera>
+                  <am3d:pos x="0" y="0" z="60127246"/>
+                  <am3d:up dx="0" dy="36000000" dz="0"/>
+                  <am3d:lookAt x="0" y="0" z="0"/>
+                  <am3d:perspective fov="2700000"/>
+                </am3d:camera>
+                <am3d:trans>
+                  <am3d:meterPerModelUnit n="338231" d="1000000"/>
+                  <am3d:preTrans dx="0" dy="-12947221" dz="-6575"/>
+                  <am3d:scale>
+                    <am3d:sx n="1000000" d="1000000"/>
+                    <am3d:sy n="1000000" d="1000000"/>
+                    <am3d:sz n="1000000" d="1000000"/>
+                  </am3d:scale>
+                  <am3d:rot/>
+                  <am3d:postTrans dx="0" dy="0" dz="0"/>
+                </am3d:trans>
+                <am3d:raster rName="Office3DRenderer" rVer="16.0.8326">
+                  <am3d:blip r:embed="rId4"/>
+                </am3d:raster>
+                <am3d:objViewport viewportSz="2700867"/>
+                <am3d:ambientLight>
+                  <am3d:clr>
+                    <a:scrgbClr r="50000" g="50000" b="50000"/>
+                  </am3d:clr>
+                  <am3d:illuminance n="500000" d="1000000"/>
+                </am3d:ambientLight>
+                <am3d:ptLight rad="0">
+                  <am3d:clr>
+                    <a:scrgbClr r="100000" g="75000" b="50000"/>
+                  </am3d:clr>
+                  <am3d:intensity n="9765625" d="1000000"/>
+                  <am3d:pos x="21959998" y="70920001" z="16344003"/>
+                </am3d:ptLight>
+                <am3d:ptLight rad="0">
+                  <am3d:clr>
+                    <a:scrgbClr r="40000" g="60000" b="95000"/>
+                  </am3d:clr>
+                  <am3d:intensity n="12250000" d="1000000"/>
+                  <am3d:pos x="-37964106" y="51130435" z="57631972"/>
+                </am3d:ptLight>
+                <am3d:ptLight rad="0">
+                  <am3d:clr>
+                    <a:scrgbClr r="86837" g="72700" b="100000"/>
+                  </am3d:clr>
+                  <am3d:intensity n="3125000" d="1000000"/>
+                  <am3d:pos x="-37739122" y="58056624" z="-34769649"/>
+                </am3d:ptLight>
+              </am3d:model3d>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="4" name="mqtt://iot.digivis.se/datadirectory/TestArea/TestFiles/monkey.glb">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7D9A5B7-D57E-02FA-75CB-B9F1C91C95C2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noGrp="1" noRot="1" noChangeAspect="1" noMove="1" noResize="1" noEditPoints="1" noAdjustHandles="1" noChangeArrowheads="1" noChangeShapeType="1" noCrop="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="533400" y="5372100"/>
+              <a:ext cx="1885950" cy="1409700"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>492794</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12242</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="mqtt://iot.digivis.se/datadirectory/TestArea/TestFiles/312961D0.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50F91E7D-E8AD-B93B-D613-0B0FEA46127E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4876800" y="1143001"/>
+          <a:ext cx="2931194" cy="3060241"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -828,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="H5:R82"/>
+  <dimension ref="I6:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="T59" sqref="T59"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,71 +1020,136 @@
     <col min="12" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H5" t="str" cm="1">
-        <f t="array" ref="H5">_xll.GetSelectedServerName()</f>
-        <v>iot.digivis.se</v>
-      </c>
-    </row>
-    <row r="18" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I6" t="str" cm="1">
+        <f t="array" ref="I6">_xll.get_from_dataspace(I18&amp;"312961D0.jpg")</f>
+        <v>Image 'mqtt://iot.digivis.se/datadirectory/TestArea/TestFiles/312961D0.jpg' is already up to date. (hash match)</v>
+      </c>
+    </row>
+    <row r="8" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I8" t="str" cm="1">
+        <f t="array" ref="I8">_xll.get_from_dataspace(I18&amp;"monkey.glb")</f>
+        <v>3D model shape 'mqtt://iot.digivis.se/datadirectory/TestArea/TestFiles/monkey.glb' is already up to date.</v>
+      </c>
+    </row>
+    <row r="12" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I12" t="b" cm="1">
+        <f t="array" ref="I12">_xll.checkworkbookhashandupdate("test","test2")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="V13" t="str" cm="1">
+        <f t="array" ref="V13:V26">_xll.get_hash_keys()</f>
+        <v>MSIP_Label_680afd86-dcf7-4483-b9eb-5af1dcd104e1_Enabled</v>
+      </c>
+    </row>
+    <row r="14" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="V14" t="str">
+        <v>MSIP_Label_680afd86-dcf7-4483-b9eb-5af1dcd104e1_SetDate</v>
+      </c>
+    </row>
+    <row r="15" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="V15" t="str">
+        <v>MSIP_Label_680afd86-dcf7-4483-b9eb-5af1dcd104e1_Method</v>
+      </c>
+    </row>
+    <row r="16" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="V16" t="str">
+        <v>MSIP_Label_680afd86-dcf7-4483-b9eb-5af1dcd104e1_Name</v>
+      </c>
+    </row>
+    <row r="17" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="V17" t="str">
+        <v>MSIP_Label_680afd86-dcf7-4483-b9eb-5af1dcd104e1_SiteId</v>
+      </c>
+    </row>
+    <row r="18" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I18" t="str" cm="1">
-        <f t="array" ref="I18:I82">_xll.get_from_dataspace("mqtt://iot.digivis.se/datadirectory/TestArea/TestFiles/")</f>
+        <f t="array" ref="I18:I89">_xll.get_from_dataspace("mqtt://iot.digivis.se/datadirectory/TestArea/TestFiles/")</f>
         <v>mqtt://iot.digivis.se/datadirectory/TestArea/TestFiles/</v>
       </c>
-    </row>
-    <row r="19" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="V18" t="str">
+        <v>MSIP_Label_680afd86-dcf7-4483-b9eb-5af1dcd104e1_ActionId</v>
+      </c>
+    </row>
+    <row r="19" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I19" t="str">
         <v>📁 .BoxTextured.glb/</v>
       </c>
-    </row>
-    <row r="20" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="V19" t="str">
+        <v>MSIP_Label_680afd86-dcf7-4483-b9eb-5af1dcd104e1_ContentBits</v>
+      </c>
+    </row>
+    <row r="20" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I20" t="str">
         <v>📁 .Charlotte Runberg(3).jpeg/</v>
       </c>
-    </row>
-    <row r="21" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="V20" t="str">
+        <v>MSIP_Label_680afd86-dcf7-4483-b9eb-5af1dcd104e1_Tag</v>
+      </c>
+    </row>
+    <row r="21" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I21" t="str">
         <v>📁 .Charlotte Runberg(5).jpeg/</v>
       </c>
-    </row>
-    <row r="22" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="V21" t="str">
+        <v>C:\Users\anton\AppData\Local\Temp\dataspace_cache\1540689257679418022.jpg</v>
+      </c>
+    </row>
+    <row r="22" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I22" t="str">
         <v>📁 .Charlotte Runberg(6).jpeg/</v>
       </c>
-    </row>
-    <row r="23" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="V22" t="str">
+        <v>C:\Users\anton\AppData\Local\Temp\dataspace_cache\2273265183511553736.jpg</v>
+      </c>
+    </row>
+    <row r="23" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I23" t="str">
+        <v>📁 .D05.02 Public report on the LDT toolbox detailed specifications.pdf/</v>
+      </c>
+      <c r="V23" t="str">
+        <v>C:\Users\anton\AppData\Local\Temp\dataspace_cache\322079861342373506.jpg</v>
+      </c>
+    </row>
+    <row r="24" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I24" t="str">
         <v>📁 .Formula.json/</v>
       </c>
-    </row>
-    <row r="24" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I24" t="str">
+      <c r="V24" t="str">
+        <v>C:\Users\anton\AppData\Local\Temp\dataspace_cache\10308b38f781de867a9a5ed8f17ffaf21d856a67c3b0b156418f2a778f477d2b.jpg</v>
+      </c>
+    </row>
+    <row r="25" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I25" t="str">
         <v>📁 .MyExport.glb/</v>
       </c>
-    </row>
-    <row r="25" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I25" t="str">
+      <c r="V25" t="str">
+        <v>test</v>
+      </c>
+    </row>
+    <row r="26" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I26" t="str">
         <v>📁 .MyExport2.glb/</v>
       </c>
-    </row>
-    <row r="26" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I26" t="str">
+      <c r="V26" t="str">
+        <v>C:\Users\anton\AppData\Local\Temp\dataspace_cache\123990d115b9ce3e1b8a66eb257962e7f0c465969ffbd051d3f4ff30c8781cd9.glb</v>
+      </c>
+    </row>
+    <row r="27" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I27" t="str">
         <v>📁 .johan.glb/</v>
       </c>
     </row>
-    <row r="27" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I27" t="str">
+    <row r="28" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I28" t="str">
         <v>📁 .johan2.glb/</v>
       </c>
     </row>
-    <row r="28" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I28" t="str">
+    <row r="29" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I29" t="str">
         <v>📁 .johantest.glb/</v>
-      </c>
-    </row>
-    <row r="29" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I29" t="str">
-        <v>📁 .monkey.glb/</v>
       </c>
       <c r="M29" t="str">
         <f>HYPERLINK("https://www.google.com", "Google")</f>
@@ -916,68 +1161,68 @@
       </c>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I30" t="str">
+        <v>📁 .monkey.glb/</v>
+      </c>
+    </row>
+    <row r="31" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I31" t="str">
         <v>📁 .multiobject.glb/</v>
       </c>
     </row>
-    <row r="31" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I31" t="str">
+    <row r="32" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I32" t="str">
         <v>📁 .ortofoto_wgs84_proxy_kista (1).png/</v>
-      </c>
-    </row>
-    <row r="32" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I32" t="str">
-        <v>📁 .test1.json/</v>
       </c>
     </row>
     <row r="33" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I33" t="str">
-        <v>📁 1:1/</v>
+        <v>📁 .test1.json/</v>
       </c>
     </row>
     <row r="34" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I34" t="str">
-        <v>📁 1:1 (1)/</v>
+        <v>📁 1:1/</v>
       </c>
     </row>
     <row r="35" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I35" t="str">
-        <v>📄 210701521070152107015hej.txt</v>
+        <v>📁 1:1 (1)/</v>
       </c>
     </row>
     <row r="36" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I36" t="str">
-        <v>📄 312961D0.jpg</v>
+        <v>📄 210701521070152107015hej.txt</v>
       </c>
     </row>
     <row r="37" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I37" t="str">
-        <v>📄 312961D2.jpg</v>
+        <v>📄 312961D0.jpg</v>
       </c>
     </row>
     <row r="38" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I38" t="str">
-        <v>📄 312961D3.jpg</v>
+        <v>📄 312961D2.jpg</v>
       </c>
       <c r="M38" t="str">
         <f>I18&amp;I40</f>
-        <v>mqtt://iot.digivis.se/datadirectory/TestArea/TestFiles/📄 Array.json</v>
+        <v>mqtt://iot.digivis.se/datadirectory/TestArea/TestFiles/📄 312961D5.jpg</v>
       </c>
     </row>
     <row r="39" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I39" t="str">
-        <v>📄 312961D5.jpg</v>
+        <v>📄 312961D3.jpg</v>
       </c>
     </row>
     <row r="40" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I40" t="str">
-        <v>📄 Array.json</v>
+        <v>📄 312961D5.jpg</v>
       </c>
     </row>
     <row r="41" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I41" t="str">
-        <v>📄 BoxTextured.glb</v>
+        <v>📄 Array.json</v>
       </c>
       <c r="M41" t="s">
         <v>0</v>
@@ -985,37 +1230,37 @@
     </row>
     <row r="42" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I42" t="str">
-        <v>📄 Charlotte Runberg(3).jpeg</v>
+        <v>📄 Bild1.png</v>
       </c>
     </row>
     <row r="43" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I43" t="str">
-        <v>📄 Charlotte Runberg(5).jpeg</v>
+        <v>📄 BoxTextured.glb</v>
       </c>
     </row>
     <row r="44" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I44" t="str">
-        <v>📄 Charlotte Runberg(6).jpeg</v>
+        <v>📄 Charlotte Runberg(3).jpeg</v>
       </c>
     </row>
     <row r="45" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I45" t="str">
-        <v>📄 D05.02 Public report on the LDT toolbox detailed specifications.pdf</v>
+        <v>📄 Charlotte Runberg(5).jpeg</v>
       </c>
     </row>
     <row r="46" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I46" t="str">
-        <v>📄 Duck.glb</v>
+        <v>📄 Charlotte Runberg(6).jpeg</v>
       </c>
     </row>
     <row r="47" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I47" t="str">
-        <v>📄 Formula.json</v>
+        <v>📄 D05.02 Public report on the LDT toolbox detailed specifications.pdf</v>
       </c>
     </row>
     <row r="48" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I48" t="str">
-        <v>📁 GoogleTiles/</v>
+        <v>📄 Duck.glb</v>
       </c>
       <c r="P48" t="s">
         <v>1</v>
@@ -1023,12 +1268,12 @@
     </row>
     <row r="49" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I49" t="str">
-        <v>📁 Linktest/</v>
+        <v>📄 Formula.json</v>
       </c>
     </row>
     <row r="50" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I50" t="str">
-        <v>📄 MyExport.glb</v>
+        <v>📁 GoogleTiles/</v>
       </c>
       <c r="P50" s="1" t="s">
         <v>2</v>
@@ -1036,46 +1281,46 @@
     </row>
     <row r="51" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I51" t="str">
-        <v>📄 MyExport2.glb</v>
+        <v>📁 Linktest/</v>
       </c>
     </row>
     <row r="52" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I52" t="str">
-        <v>📄 Object view.svg</v>
+        <v>📄 MyExport.glb</v>
       </c>
     </row>
     <row r="53" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I53" t="str">
-        <v>📄 Readme.md</v>
+        <v>📄 MyExport2.glb</v>
       </c>
     </row>
     <row r="54" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I54" t="str">
-        <v>📁 Skull/</v>
+        <v>📄 Object view.svg</v>
       </c>
     </row>
     <row r="55" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I55" t="str">
-        <v>📄 XAM_steel_7011.unity3d</v>
+        <v>📄 Readme.md</v>
       </c>
     </row>
     <row r="56" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I56" t="str">
-        <v>📁 blue-flower-animated/</v>
+        <v>📁 Skull/</v>
       </c>
       <c r="L56" t="str" cm="1">
         <f t="array" ref="L56">_xll.rotera_figur("Grupp 11",L59)</f>
-        <v>Figuren 'Grupp 11' är nu roterad -104.01428571428572°</v>
+        <v>Figuren 'Grupp 11' är nu roterad -106.15714285714286°</v>
       </c>
     </row>
     <row r="57" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I57" t="str">
-        <v>📁 buildings/</v>
+        <v>📄 XAM_steel_7011.unity3d</v>
       </c>
     </row>
     <row r="58" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I58" t="str">
-        <v>📄 cloud.png</v>
+        <v>📄 YQY4Sfx.png</v>
       </c>
       <c r="L58">
         <v>-150</v>
@@ -1083,133 +1328,168 @@
     </row>
     <row r="59" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I59" t="str">
-        <v>📄 direct.glb</v>
+        <v>📁 blue-flower-animated/</v>
       </c>
       <c r="L59">
         <f>(L62/7000)*300 -150</f>
-        <v>-104.01428571428572</v>
+        <v>-106.15714285714286</v>
       </c>
     </row>
     <row r="60" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I60" t="str">
-        <v>📁 fastigheter/</v>
+        <v>📁 buildings/</v>
       </c>
     </row>
     <row r="61" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I61" t="str">
-        <v>📄 fromdisk.glb</v>
+        <v>📄 cloud.png</v>
       </c>
     </row>
     <row r="62" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I62" t="str">
-        <v>📄 fromdisk2.glb</v>
+        <v>📄 direct.glb</v>
       </c>
       <c r="L62" cm="1">
         <f t="array" ref="L62">_xll.subscribe_livedata("mqtt://iot.digivis.se/datadirectory/TestArea/signalA[power]")</f>
-        <v>1073</v>
+        <v>1023</v>
       </c>
       <c r="M62" t="str">
         <f>L62&amp; " W"</f>
-        <v>1073 W</v>
+        <v>1023 W</v>
       </c>
     </row>
     <row r="63" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I63" t="str">
-        <v>📄 hej.txt</v>
+        <v>📁 fastigheter/</v>
       </c>
     </row>
     <row r="64" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I64" t="str">
-        <v>📄 hus.glb</v>
+        <v>📄 fromdisk.glb</v>
       </c>
     </row>
     <row r="65" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I65" t="str">
-        <v>📄 johan.glb</v>
+        <v>📄 fromdisk2.glb</v>
       </c>
     </row>
     <row r="66" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I66" t="str">
-        <v>📄 johan2.glb</v>
+        <v>📄 hej.txt</v>
       </c>
     </row>
     <row r="67" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I67" t="str">
-        <v>📄 johans_assetbundle.unity3d</v>
+        <v>📄 hus.glb</v>
       </c>
     </row>
     <row r="68" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I68" t="str">
-        <v>📄 johantest.glb</v>
+        <v>📄 image001.jpg</v>
       </c>
     </row>
     <row r="69" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I69" t="str">
-        <v>📁 kommuner/</v>
+        <v>📄 johan.glb</v>
       </c>
     </row>
     <row r="70" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I70" t="str">
-        <v>📄 komuner.unity3d</v>
+        <v>📄 johan2.glb</v>
       </c>
     </row>
     <row r="71" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I71" t="str">
-        <v>📄 meshyai.glb</v>
+        <v>📄 johans_assetbundle.unity3d</v>
       </c>
     </row>
     <row r="72" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I72" t="str">
-        <v>📄 monkey.glb</v>
+        <v>📄 johantest.glb</v>
       </c>
     </row>
     <row r="73" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I73" t="str">
-        <v>📄 move_files.py</v>
+        <v>📁 kommuner/</v>
       </c>
     </row>
     <row r="74" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I74" t="str">
-        <v>📄 multiobject.glb</v>
+        <v>📄 komuner.unity3d</v>
       </c>
     </row>
     <row r="75" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I75" t="str">
-        <v>📄 ortofoto_wgs84_proxy_kista (1).png</v>
+        <v>📄 meshyai.glb</v>
       </c>
     </row>
     <row r="76" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I76" t="str">
-        <v>📄 skull_downloadable.glb</v>
+        <v>📄 monkey.glb</v>
       </c>
     </row>
     <row r="77" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I77" t="str">
-        <v>📄 steampunk_underwater_explorer.glb</v>
+        <v>📄 move_files.py</v>
       </c>
     </row>
     <row r="78" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I78" t="str">
-        <v>📄 steampunk_underwater_explorer_1k_texture.glb</v>
+        <v>📄 ms-teams_Mt0xVtYsBH.png</v>
       </c>
     </row>
     <row r="79" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I79" t="str">
-        <v>📄 t#hej.txt</v>
+        <v>📄 multiobject.glb</v>
       </c>
     </row>
     <row r="80" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I80" t="str">
-        <v>📄 temp.svg</v>
+        <v>📄 ortofoto_wgs84_proxy_kista (1).png</v>
       </c>
     </row>
     <row r="81" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I81" t="str">
-        <v>📄 test1.json</v>
+        <v>📄 skull_downloadable.glb</v>
       </c>
     </row>
     <row r="82" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I82" t="str">
+        <v>📄 steampunk_underwater_explorer.glb</v>
+      </c>
+    </row>
+    <row r="83" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I83" t="str">
+        <v>📄 steampunk_underwater_explorer_1k_texture.glb</v>
+      </c>
+    </row>
+    <row r="84" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I84" t="str">
+        <v>📄 stream-icon-samples.svg</v>
+      </c>
+    </row>
+    <row r="85" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I85" t="str">
+        <v>📄 t#hej.txt</v>
+      </c>
+    </row>
+    <row r="86" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I86" t="str">
+        <v>📄 temp.svg</v>
+      </c>
+    </row>
+    <row r="87" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I87" t="str">
+        <v>📄 test.json</v>
+      </c>
+    </row>
+    <row r="88" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I88" t="str">
+        <v>📄 test1.json</v>
+      </c>
+    </row>
+    <row r="89" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I89" t="str">
         <v>📄 testpin.unity3d</v>
       </c>
     </row>

</xml_diff>